<commit_message>
New portal added: bund.de
</commit_message>
<xml_diff>
--- a/CF_Public_Tender_Research/Data/Portale.xlsx
+++ b/CF_Public_Tender_Research/Data/Portale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrose\Documents\UiPath\CF_Public_Tender_Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Entwicklung\CF internes Projekt - Portalsuche\CF_Public_Tender_Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>BMWI</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Bund</t>
+  </si>
+  <si>
+    <t>https://www.service.bund.de/Content/DE/Ausschreibungen/Suche/Formular.html?resultsPerPage=20</t>
   </si>
 </sst>
 </file>
@@ -385,16 +391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="94" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -453,12 +459,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Changed the URL of service.bund.de
</commit_message>
<xml_diff>
--- a/CF_Public_Tender_Research/Data/Portale.xlsx
+++ b/CF_Public_Tender_Research/Data/Portale.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrose\Documents\Github\CF Portal Search\CF_Public_Tender_Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Entwicklung\CF internes Projekt - Portalsuche\CF_Public_Tender_Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33660" windowHeight="15540"/>
+    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="33660" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="öffentliche Portale" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <t>Bund</t>
   </si>
   <si>
-    <t>https://www.service.bund.de/Content/DE/Ausschreibungen/Suche/Formular.html?resultsPerPage=20</t>
+    <t>https://www.service.bund.de/</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,6 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>